<commit_message>
點字印表機增加 viewplus.com 的 VP columbia 2。
</commit_message>
<xml_diff>
--- a/Doc/行銷/客戶資料/客戶資料.xlsx
+++ b/Doc/行銷/客戶資料/客戶資料.xlsx
@@ -1,28 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\視覺輔助\text-to-braille\Doc\行銷\客戶資料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB95D81-78C2-4DC6-8D27-85ABB60F07B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469EC9E0-E2BB-4928-BC46-B0139AB2AB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>嘉義市崇文國民小學</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -228,6 +240,18 @@
   </si>
   <si>
     <t>19CE-141B-2270-1C55</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1FD4-2332-1A6F-054A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宇崝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>忘記何時給的序號，以及是否付費。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -980,7 +1004,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1276,15 +1300,21 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="18.600000000000001" customHeight="1">
-      <c r="A15" s="11"/>
+      <c r="A15" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
+      <c r="C15" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="11"/>
       <c r="G15" s="9"/>
       <c r="H15" s="15"/>
-      <c r="I15" s="11"/>
+      <c r="I15" s="11" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="18.600000000000001" customHeight="1">
       <c r="A16" s="11"/>

</xml_diff>